<commit_message>
Update Infosys internship artifacts
</commit_message>
<xml_diff>
--- a/Internship_artifacts/Defect_Tracker Template_v0.1.xlsx
+++ b/Internship_artifacts/Defect_Tracker Template_v0.1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://infosystechnologies-my.sharepoint.com/personal/kamaljeet_kaur01_ad_infosys_com1/Documents/Infosys/CC/Events/Oct 2021 - Mar 2022/CC2.0/Internship/Jan-Apr 2022/Artifacts/internship/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ankitha B M\OneDrive\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="22" documentId="13_ncr:101_{A9B59A9A-789B-4A89-A90D-BB9A1B756E8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1529751A-99C4-4233-8104-CEB3E356847C}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7D8B424-F8D6-42AA-AE7A-C414EF5958BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Defects" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="85">
   <si>
     <t>Sl No</t>
   </si>
@@ -69,6 +69,213 @@
   </si>
   <si>
     <t>Status(Open/Closed)</t>
+  </si>
+  <si>
+    <t>Sprint 1</t>
+  </si>
+  <si>
+    <t>Configuration</t>
+  </si>
+  <si>
+    <t>Closed</t>
+  </si>
+  <si>
+    <t>Validation</t>
+  </si>
+  <si>
+    <t>Sprint 2</t>
+  </si>
+  <si>
+    <t>UI Defect</t>
+  </si>
+  <si>
+    <t>Logic Defect</t>
+  </si>
+  <si>
+    <t>Sprint 3</t>
+  </si>
+  <si>
+    <t>Performance</t>
+  </si>
+  <si>
+    <t>Ankitha BM</t>
+  </si>
+  <si>
+    <t>CORS issue while accessing backend APIs from frontend</t>
+  </si>
+  <si>
+    <t>Enabled CORS in backend</t>
+  </si>
+  <si>
+    <t>Yellu Harshitha Reddy</t>
+  </si>
+  <si>
+    <t>Login API accepts empty credentials</t>
+  </si>
+  <si>
+    <t>Snehalatha Reddy</t>
+  </si>
+  <si>
+    <t>Added input validation</t>
+  </si>
+  <si>
+    <t>User profile data not saved correctly</t>
+  </si>
+  <si>
+    <t>Data Handling</t>
+  </si>
+  <si>
+    <t>Fixed JSON storage logic</t>
+  </si>
+  <si>
+    <t>Arjun Rankela</t>
+  </si>
+  <si>
+    <t>Agents not invoked correctly via LangChain</t>
+  </si>
+  <si>
+    <t>Deepak Kumar Hota</t>
+  </si>
+  <si>
+    <t>Corrected agent invocation flow</t>
+  </si>
+  <si>
+    <t>Integration</t>
+  </si>
+  <si>
+    <t>Updated orchestration logic</t>
+  </si>
+  <si>
+    <t>Subhash J</t>
+  </si>
+  <si>
+    <t>Sagar Gowd</t>
+  </si>
+  <si>
+    <t>Memory Issue</t>
+  </si>
+  <si>
+    <t>Implemented shared memory</t>
+  </si>
+  <si>
+    <t>Delay in Groq LLM API response</t>
+  </si>
+  <si>
+    <t>Added timeout handling</t>
+  </si>
+  <si>
+    <t>Palak Mehla</t>
+  </si>
+  <si>
+    <t>Wellness plan markdown not rendered properly</t>
+  </si>
+  <si>
+    <t>Sprint 4</t>
+  </si>
+  <si>
+    <t>Karthik Bhandarkar</t>
+  </si>
+  <si>
+    <t>Fixed markdown rendering</t>
+  </si>
+  <si>
+    <t>Page refresh causes UI break</t>
+  </si>
+  <si>
+    <t>UI / Routing</t>
+  </si>
+  <si>
+    <t>Fixed routing logic</t>
+  </si>
+  <si>
+    <t>Komali Priya Mokkapati</t>
+  </si>
+  <si>
+    <t>Error messages not user-friendly</t>
+  </si>
+  <si>
+    <t>UX Defect</t>
+  </si>
+  <si>
+    <t>Improved error messages</t>
+  </si>
+  <si>
+    <t>Chhavi</t>
+  </si>
+  <si>
+    <t>Invalid follow-up input not handled</t>
+  </si>
+  <si>
+    <t>Added follow-up validation</t>
+  </si>
+  <si>
+    <t>Hemangi Borase</t>
+  </si>
+  <si>
+    <t>UI Enhancement</t>
+  </si>
+  <si>
+    <t>Added loading spinner</t>
+  </si>
+  <si>
+    <t>Abhilash KR</t>
+  </si>
+  <si>
+    <t>Logging</t>
+  </si>
+  <si>
+    <t>Improved logging messages</t>
+  </si>
+  <si>
+    <t>Issue resolved</t>
+  </si>
+  <si>
+    <t>Validation successful</t>
+  </si>
+  <si>
+    <t>Data persistence verified</t>
+  </si>
+  <si>
+    <t>Agents working as expected</t>
+  </si>
+  <si>
+    <t>Orchestrator not combining agent outputs properly</t>
+  </si>
+  <si>
+    <t>Unified response generated</t>
+  </si>
+  <si>
+    <t>Follow-up questions losing previous context</t>
+  </si>
+  <si>
+    <t>Context retained</t>
+  </si>
+  <si>
+    <t>Performance improved</t>
+  </si>
+  <si>
+    <t>UI rendering fixed</t>
+  </si>
+  <si>
+    <t>Navigation stable</t>
+  </si>
+  <si>
+    <t>Better user experience</t>
+  </si>
+  <si>
+    <t>Edge case handled</t>
+  </si>
+  <si>
+    <t>Loading indicator missing during API calls</t>
+  </si>
+  <si>
+    <t>UX improvement</t>
+  </si>
+  <si>
+    <t>Backend logs insufficient during failures</t>
+  </si>
+  <si>
+    <t>Easier debugging</t>
   </si>
 </sst>
 </file>
@@ -174,7 +381,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -191,6 +398,12 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -209,9 +422,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -249,9 +462,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -284,26 +497,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -336,26 +532,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -531,25 +710,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="17.54296875" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" style="4" customWidth="1"/>
-    <col min="4" max="4" width="42.140625" style="4" customWidth="1"/>
+    <col min="1" max="1" width="6.1796875" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.453125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.453125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="42.1796875" style="4" customWidth="1"/>
     <col min="5" max="5" width="16" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="10" width="21.85546875" style="4" customWidth="1"/>
-    <col min="11" max="11" width="16.85546875" style="4" customWidth="1"/>
-    <col min="12" max="16384" width="17.5703125" style="4"/>
+    <col min="6" max="6" width="12.54296875" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.54296875" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="10" width="21.81640625" style="4" customWidth="1"/>
+    <col min="11" max="11" width="16.81640625" style="4" customWidth="1"/>
+    <col min="12" max="16384" width="17.54296875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="2" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" s="2" customFormat="1" ht="31" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -584,176 +763,462 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-    </row>
-    <row r="3" spans="1:11" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
-    </row>
-    <row r="4" spans="1:11" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
-    </row>
-    <row r="5" spans="1:11" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
-    </row>
-    <row r="6" spans="1:11" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
-    </row>
-    <row r="7" spans="1:11" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="6"/>
-    </row>
-    <row r="8" spans="1:11" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
-    </row>
-    <row r="9" spans="1:11" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A9" s="5"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
-      <c r="K9" s="6"/>
-    </row>
-    <row r="10" spans="1:11" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="6"/>
-    </row>
-    <row r="11" spans="1:11" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A11" s="3"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
-      <c r="K11" s="3"/>
-    </row>
-    <row r="12" spans="1:11" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A12" s="5"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
-      <c r="K12" s="6"/>
-    </row>
-    <row r="13" spans="1:11" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A13" s="3"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
-      <c r="J13" s="3"/>
-      <c r="K13" s="3"/>
-    </row>
-    <row r="14" spans="1:11" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A14" s="5"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
-      <c r="J14" s="3"/>
-      <c r="K14" s="6"/>
-    </row>
-    <row r="15" spans="1:11" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" ht="26" x14ac:dyDescent="0.3">
+      <c r="A2" s="8">
+        <v>1</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="9">
+        <v>45995</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="I2" s="9">
+        <v>45996</v>
+      </c>
+      <c r="J2" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="K2" s="8" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="26" x14ac:dyDescent="0.3">
+      <c r="A3" s="8">
+        <v>2</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="9">
+        <v>45996</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="I3" s="9">
+        <v>45997</v>
+      </c>
+      <c r="J3" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="K3" s="8" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="26" x14ac:dyDescent="0.3">
+      <c r="A4" s="8">
+        <v>3</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="9">
+        <v>45997</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="I4" s="9">
+        <v>45997</v>
+      </c>
+      <c r="J4" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="K4" s="8" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="26" x14ac:dyDescent="0.3">
+      <c r="A5" s="8">
+        <v>4</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" s="9">
+        <v>45997</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="I5" s="9">
+        <v>45998</v>
+      </c>
+      <c r="J5" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="K5" s="8" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="26" x14ac:dyDescent="0.3">
+      <c r="A6" s="8">
+        <v>5</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" s="9">
+        <v>45998</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="I6" s="9">
+        <v>45999</v>
+      </c>
+      <c r="J6" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="K6" s="8" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="26" x14ac:dyDescent="0.3">
+      <c r="A7" s="8">
+        <v>6</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7" s="9">
+        <v>45998</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="H7" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="I7" s="9">
+        <v>45999</v>
+      </c>
+      <c r="J7" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="K7" s="8" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="26" x14ac:dyDescent="0.3">
+      <c r="A8" s="8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="C8" s="9">
+        <v>45999</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="H8" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="I8" s="9">
+        <v>46000</v>
+      </c>
+      <c r="J8" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="K8" s="8" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="26" x14ac:dyDescent="0.3">
+      <c r="A9" s="8">
+        <v>8</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C9" s="9">
+        <v>46000</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="H9" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="I9" s="9">
+        <v>46001</v>
+      </c>
+      <c r="J9" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="K9" s="8" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="26" x14ac:dyDescent="0.3">
+      <c r="A10" s="8">
+        <v>9</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C10" s="9">
+        <v>46001</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="H10" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="I10" s="9">
+        <v>46002</v>
+      </c>
+      <c r="J10" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="K10" s="8" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="26" x14ac:dyDescent="0.3">
+      <c r="A11" s="8">
+        <v>10</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="C11" s="9">
+        <v>46001</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="H11" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="I11" s="9">
+        <v>46002</v>
+      </c>
+      <c r="J11" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="K11" s="8" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="26" x14ac:dyDescent="0.3">
+      <c r="A12" s="8">
+        <v>11</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="C12" s="9">
+        <v>46001</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="H12" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="I12" s="9">
+        <v>46002</v>
+      </c>
+      <c r="J12" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="K12" s="8" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="26" x14ac:dyDescent="0.3">
+      <c r="A13" s="8">
+        <v>12</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="C13" s="9">
+        <v>46002</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="G13" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="H13" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="I13" s="9">
+        <v>46002</v>
+      </c>
+      <c r="J13" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="K13" s="8" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A14" s="8">
+        <v>13</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="C14" s="9">
+        <v>46002</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="G14" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="H14" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="I14" s="9">
+        <v>46002</v>
+      </c>
+      <c r="J14" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="K14" s="8" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="15.5" x14ac:dyDescent="0.3">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -766,7 +1231,7 @@
       <c r="J15" s="3"/>
       <c r="K15" s="3"/>
     </row>
-    <row r="16" spans="1:11" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" ht="15.5" x14ac:dyDescent="0.3">
       <c r="A16" s="5"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
@@ -779,7 +1244,7 @@
       <c r="J16" s="3"/>
       <c r="K16" s="6"/>
     </row>
-    <row r="17" spans="1:11" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" ht="15.5" x14ac:dyDescent="0.3">
       <c r="A17" s="5"/>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
@@ -792,7 +1257,7 @@
       <c r="J17" s="3"/>
       <c r="K17" s="6"/>
     </row>
-    <row r="18" spans="1:11" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" ht="15.5" x14ac:dyDescent="0.3">
       <c r="A18" s="5"/>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
@@ -805,7 +1270,7 @@
       <c r="J18" s="3"/>
       <c r="K18" s="6"/>
     </row>
-    <row r="19" spans="1:11" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" ht="15.5" x14ac:dyDescent="0.3">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
@@ -818,7 +1283,7 @@
       <c r="J19" s="3"/>
       <c r="K19" s="3"/>
     </row>
-    <row r="20" spans="1:11" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" ht="15.5" x14ac:dyDescent="0.3">
       <c r="A20" s="5"/>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
@@ -843,7 +1308,7 @@
           <x14:formula1>
             <xm:f>Sheet2!$A$1:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>G1:G1048576</xm:sqref>
+          <xm:sqref>G1 G15:G1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -859,29 +1324,29 @@
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>14</v>
       </c>
@@ -893,6 +1358,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F50FC49184C87E449886FB52439922C9" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="f85b7e58c3d8889ba0673e7b34a193a6">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b67b99c0-208c-4860-83e0-51466af787c4" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5d43477c1ade21a66d9a75ba2d5aa042" ns2:_="">
     <xsd:import namespace="b67b99c0-208c-4860-83e0-51466af787c4"/>
@@ -1024,12 +1495,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -1040,6 +1505,15 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8B149665-BEBB-4C97-BAA6-72374EAA67F9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{191CB444-B9BF-4C91-94BD-600524521497}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1057,15 +1531,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8B149665-BEBB-4C97-BAA6-72374EAA67F9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{20D196DE-5AC8-4D3B-8CD7-1A2AE6EEDD72}">
   <ds:schemaRefs>

</xml_diff>